<commit_message>
Aspect-dependent melt factor is working in C++.
</commit_message>
<xml_diff>
--- a/tests/resources/glacier snowpack.xlsx
+++ b/tests/resources/glacier snowpack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\hydrobricks\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB8A484-DC81-4E3F-8530-04335A9E566A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05110CA-C065-41DE-8A73-6AC2F69A95AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="18900" windowHeight="10830" activeTab="1" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
+    <workbookView xWindow="28995" yWindow="255" windowWidth="27630" windowHeight="14100" activeTab="1" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
   </bookViews>
   <sheets>
     <sheet name="model 1" sheetId="2" r:id="rId1"/>
@@ -880,7 +880,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1214,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="3"/>
+        <f>I15+E16-H16</f>
         <v>7</v>
       </c>
       <c r="J16" s="2">
@@ -1247,6 +1247,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="2">
+        <f>I16+E17-H17</f>
         <v>0</v>
       </c>
       <c r="J17" s="2">

</xml_diff>